<commit_message>
+ I moved some of the {OS}_defs*.f90 files into the NWTC Library sys*.f90 files. + I created a mesh for inputs and outputs on the platform reference point in ElastoDyn, replacing variable PtfmFt.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@384 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: b844da865e8885befacbf64ef096e6a5094f1c8e
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21390" windowHeight="9570" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15240" windowHeight="7965" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -7038,9 +7038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7157,9 +7155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G930"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22402,7 +22398,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -23013,7 +23009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G888"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -37571,7 +37567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
fixed minor details in screen/file output. updated version numbers for consistency added test 19 with SubDyn! updated README_FAST8.docx update CertTest/Tst files with results
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@542 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 208589c9c2d7a64cd2a74cd0a3956a44ce5d51fe
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15240" windowHeight="7965" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="240" windowWidth="15240" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -6381,19 +6381,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <condense val="0"/>
@@ -6741,9 +6729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6916,7 +6902,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22123,7 +22109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
+ added lidar files + updated dependencies + updated compile scripts and codumentation
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@896 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 5d192bd72536b343926fcf94fc242197c9ce1d72
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="240" windowWidth="15240" windowHeight="7905"/>
+    <workbookView xWindow="120" yWindow="240" windowWidth="15240" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -20,12 +20,11 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">ElastoDyn!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4381" uniqueCount="2076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4406" uniqueCount="2091">
   <si>
     <t>Category</t>
   </si>
@@ -6276,6 +6275,51 @@
   </si>
   <si>
     <t>(WindVxi and uWind will be interchangable names for this channel)</t>
+  </si>
+  <si>
+    <t>Nacelle Tuned Mass Damper (TMD)</t>
+  </si>
+  <si>
+    <t>Nacelle X TMD position (displacement)</t>
+  </si>
+  <si>
+    <t>Nacelle X TMD velocity</t>
+  </si>
+  <si>
+    <t>Nacelle X TMD acceleration</t>
+  </si>
+  <si>
+    <t>Nacelle Y TMD position (displacement)</t>
+  </si>
+  <si>
+    <t>Nacelle Y TMD velocity</t>
+  </si>
+  <si>
+    <t>Nacelle Y TMD acceleration</t>
+  </si>
+  <si>
+    <t>NTMD_XQ</t>
+  </si>
+  <si>
+    <t>NTMD_XQD</t>
+  </si>
+  <si>
+    <t>NTMD_XQD2</t>
+  </si>
+  <si>
+    <t>NTMD_YQ</t>
+  </si>
+  <si>
+    <t>NTMD_YQD</t>
+  </si>
+  <si>
+    <t>NTMD_YQD2</t>
+  </si>
+  <si>
+    <t>Relative to rest position</t>
+  </si>
+  <si>
+    <t>Relative to nacelle</t>
   </si>
 </sst>
 </file>
@@ -6730,7 +6774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6771,7 +6815,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9">
         <f>COUNTA(ServoDyn!B:B)-1</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>2070</v>
@@ -21332,9 +21376,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21343,7 +21389,7 @@
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21513,6 +21559,98 @@
       </c>
       <c r="G12" s="4" t="s">
         <v>518</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>2076</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2083</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2077</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2089</v>
+      </c>
+      <c r="F14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2084</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2078</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F15" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2085</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2079</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F16" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2086</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2080</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2089</v>
+      </c>
+      <c r="F17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>2087</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2081</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F18" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2088</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2082</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F19" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+added ElastoDyn output mesh for rQ position, necessary for lidar input from Simulink (currently a hack job)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@904 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 9ac802d33ac99948652c1f3b1c9513c5078577f3
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4406" uniqueCount="2091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4398" uniqueCount="2087">
   <si>
     <t>Category</t>
   </si>
@@ -6286,34 +6286,22 @@
     <t>Nacelle X TMD velocity</t>
   </si>
   <si>
-    <t>Nacelle X TMD acceleration</t>
-  </si>
-  <si>
     <t>Nacelle Y TMD position (displacement)</t>
   </si>
   <si>
     <t>Nacelle Y TMD velocity</t>
   </si>
   <si>
-    <t>Nacelle Y TMD acceleration</t>
-  </si>
-  <si>
     <t>NTMD_XQ</t>
   </si>
   <si>
     <t>NTMD_XQD</t>
   </si>
   <si>
-    <t>NTMD_XQD2</t>
-  </si>
-  <si>
     <t>NTMD_YQ</t>
   </si>
   <si>
     <t>NTMD_YQD</t>
-  </si>
-  <si>
-    <t>NTMD_YQD2</t>
   </si>
   <si>
     <t>Relative to rest position</t>
@@ -6815,7 +6803,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9">
         <f>COUNTA(ServoDyn!B:B)-1</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>2070</v>
@@ -21376,10 +21364,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E19"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21571,13 +21559,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="D14" t="s">
         <v>2077</v>
       </c>
       <c r="E14" t="s">
-        <v>2089</v>
+        <v>2085</v>
       </c>
       <c r="F14" t="s">
         <v>261</v>
@@ -21585,13 +21573,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="D15" t="s">
         <v>2078</v>
       </c>
       <c r="E15" t="s">
-        <v>2090</v>
+        <v>2086</v>
       </c>
       <c r="F15" t="s">
         <v>491</v>
@@ -21599,58 +21587,30 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="D16" t="s">
         <v>2079</v>
       </c>
       <c r="E16" t="s">
-        <v>2090</v>
+        <v>2085</v>
       </c>
       <c r="F16" t="s">
-        <v>492</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
       <c r="D17" t="s">
         <v>2080</v>
       </c>
       <c r="E17" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="F17" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>2087</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2081</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2090</v>
-      </c>
-      <c r="F18" t="s">
         <v>491</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>2088</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2082</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2090</v>
-      </c>
-      <c r="F19" t="s">
-        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ added TMD module, coupled with ElastoDyn; existing capabilities remain unchanged, but new TMD has not been tested
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@911 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 6c95a7334907ef2dd98f61f02195ef96498fbcdf
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -21367,7 +21367,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21879,7 +21879,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated dependencies with TMD code
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@914 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: e13bbd10bdedec017f482116497d14cd0448af87
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="240" windowWidth="15240" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="300" windowWidth="15240" windowHeight="7845" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -6934,8 +6934,8 @@
   <dimension ref="A1:G888"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D324" sqref="D324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21367,7 +21367,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21879,7 +21879,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
+ updated FAST primary input files with MoorDyn option. + added Simulink interface documentation to README_FAST8.docx + updated compile scripts to run with TMD and MoorDyn modifications + Renamed FAST_Gateway folder to VisualStudio + Renamed FAST_IO.f90 to FAST_Subs.f90 because it's more accurate + added sample FEAMooring input files to archive + added logic to make TMD outputs "invalid" when not using tmd
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@925 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: ec575069eea2deeed318c6f46c61ffafd91802d4
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4398" uniqueCount="2087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4402" uniqueCount="2088">
   <si>
     <t>Category</t>
   </si>
@@ -6308,6 +6308,9 @@
   </si>
   <si>
     <t>Relative to nacelle</t>
+  </si>
+  <si>
+    <t>.not. p%CompNTMD</t>
   </si>
 </sst>
 </file>
@@ -21367,7 +21370,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="G14" sqref="G14:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21570,6 +21573,9 @@
       <c r="F14" t="s">
         <v>261</v>
       </c>
+      <c r="G14" t="s">
+        <v>2087</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -21584,6 +21590,9 @@
       <c r="F15" t="s">
         <v>491</v>
       </c>
+      <c r="G15" t="s">
+        <v>2087</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -21598,8 +21607,11 @@
       <c r="F16" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2084</v>
       </c>
@@ -21611,6 +21623,9 @@
       </c>
       <c r="F17" t="s">
         <v>491</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ added HSS brake to Simulink INTERFACE + updated Simulink documentation and added some more error checking/fix of memory leaks in SFunc (entire CertTest runs in Simulink OpenModel) + updated dependencies
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@928 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 3322a7d1ce6ae907e6c81359337fac0f8e7c77a3
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="300" windowWidth="15240" windowHeight="7845" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="300" windowWidth="15240" windowHeight="7845"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -6765,7 +6765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6937,8 +6937,8 @@
   <dimension ref="A1:G888"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D324" sqref="D324"/>
+      <pane ySplit="1" topLeftCell="A723" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B734" sqref="B734"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21369,8 +21369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
renamed AeroDyn to AeroDyn14 in preparation for AeroDyn 15
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1019 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: c2d3c70725677352295914e86d01332230ae4e6e
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="300" windowWidth="15240" windowHeight="7848" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="300" windowWidth="15240" windowHeight="7848" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
     <sheet name="ElastoDyn" sheetId="7" r:id="rId2"/>
     <sheet name="ServoDyn" sheetId="11" r:id="rId3"/>
-    <sheet name="InflowWind" sheetId="13" r:id="rId4"/>
+    <sheet name="AeroDyn 15 - draft" sheetId="18" r:id="rId4"/>
     <sheet name="Removed" sheetId="14" r:id="rId5"/>
     <sheet name="Removed - in AeroDyn later" sheetId="12" r:id="rId6"/>
     <sheet name="Removed - in InflowWind later" sheetId="16" r:id="rId7"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="2091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4440" uniqueCount="2131">
   <si>
     <t>Category</t>
   </si>
@@ -6320,6 +6320,126 @@
   </si>
   <si>
     <t>p%method == method_RK4</t>
+  </si>
+  <si>
+    <t>Some category</t>
+  </si>
+  <si>
+    <t>YawErr</t>
+  </si>
+  <si>
+    <t>SkewAng</t>
+  </si>
+  <si>
+    <t>SkewAz</t>
+  </si>
+  <si>
+    <t>RotAeroPwr</t>
+  </si>
+  <si>
+    <t>RotAeroThrst</t>
+  </si>
+  <si>
+    <t>RotAeroTrq</t>
+  </si>
+  <si>
+    <t>RotAeroCp</t>
+  </si>
+  <si>
+    <t>RotAeroCt</t>
+  </si>
+  <si>
+    <t>RotAeroCq</t>
+  </si>
+  <si>
+    <t>ThrCntAz</t>
+  </si>
+  <si>
+    <t>ThrCntRad</t>
+  </si>
+  <si>
+    <t>BlAxInd</t>
+  </si>
+  <si>
+    <t>BlTanInd</t>
+  </si>
+  <si>
+    <t>BlCl</t>
+  </si>
+  <si>
+    <t>BlCd</t>
+  </si>
+  <si>
+    <t>BlCm</t>
+  </si>
+  <si>
+    <t>BlAoA</t>
+  </si>
+  <si>
+    <t>TwAxInd</t>
+  </si>
+  <si>
+    <t>TwTanInd</t>
+  </si>
+  <si>
+    <t>TwCl</t>
+  </si>
+  <si>
+    <t>TwCd</t>
+  </si>
+  <si>
+    <t>TwCm</t>
+  </si>
+  <si>
+    <t>TwAoA</t>
+  </si>
+  <si>
+    <t>Tower aerodynamics</t>
+  </si>
+  <si>
+    <t>Blade aerodynamics</t>
+  </si>
+  <si>
+    <t>Azimuthal location of the center of thrust</t>
+  </si>
+  <si>
+    <t>Radial location of the center of thrust</t>
+  </si>
+  <si>
+    <t>Rotor power coefficient</t>
+  </si>
+  <si>
+    <t>thrust coefficient</t>
+  </si>
+  <si>
+    <t>torque coefficient</t>
+  </si>
+  <si>
+    <t>Rotor aerodynamic power</t>
+  </si>
+  <si>
+    <t>Rotor aerodynamic thrust</t>
+  </si>
+  <si>
+    <t>Rotor aerodynamic torque</t>
+  </si>
+  <si>
+    <t>azimuth of the skew (0 up)</t>
+  </si>
+  <si>
+    <t>inflow skew angle (includes pitch and yaw error)</t>
+  </si>
+  <si>
+    <t>Yaw error</t>
+  </si>
+  <si>
+    <t>Induction factors</t>
+  </si>
+  <si>
+    <t>Aerodynamic coefficients</t>
+  </si>
+  <si>
+    <t>Angle of attack</t>
   </si>
 </sst>
 </file>
@@ -6826,8 +6946,8 @@
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="D10">
-        <f>COUNTA(InflowWind!B:B)-1</f>
-        <v>3</v>
+        <f>COUNTA(#REF!)-1</f>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>2071</v>
@@ -6945,8 +7065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G889"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A727" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A685" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G736" sqref="G736"/>
     </sheetView>
   </sheetViews>
@@ -21395,7 +21515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21659,24 +21781,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -21699,87 +21821,219 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>490</v>
+        <v>2091</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>433</v>
+        <v>2092</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>1099</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1098</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>1964</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2127</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>434</v>
+        <v>2093</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>1097</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>1964</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2126</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>435</v>
+        <v>2094</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>1101</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>1096</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>1964</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+        <v>2125</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>2095</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>2096</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2097</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>2098</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>2099</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>2101</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>2104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>2105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>2107</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>2108</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>2109</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>2110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>2112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>2113</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>2114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2130</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21918,7 +22172,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22248,7 +22502,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added Pitt/Peters correction to AD 15 input files; updated dependencies and recompiled executables; added a Test 26 for BeamDyn; added NumBl and NumElementsPerBlade as return values to OpenFOAM in FAST_Library's Init and Restart routines (per request of Sang and Avi)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1113 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 911191d6f83b60ea7495cb63b5d09eec4e7b6164
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="360" windowWidth="11928" windowHeight="5364" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="420" windowWidth="11928" windowHeight="5304" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -14776,12 +14776,12 @@
         <v>2073</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>507</v>
       </c>
@@ -14789,7 +14789,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>508</v>
       </c>
@@ -14797,7 +14797,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>510</v>
       </c>
@@ -14805,7 +14805,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>513</v>
       </c>
@@ -14875,7 +14875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G889"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
@@ -15061,7 +15061,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>378</v>
       </c>
@@ -29325,7 +29325,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G354"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34428,7 +34430,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34582,7 +34584,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2065</v>
       </c>
@@ -34610,7 +34612,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>2075</v>
       </c>
@@ -34618,7 +34620,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>2080</v>
       </c>
@@ -34635,7 +34637,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>2081</v>
       </c>
@@ -34652,7 +34654,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>2082</v>
       </c>
@@ -34669,7 +34671,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2083</v>
       </c>

</xml_diff>

<commit_message>
updated with new outputs for BeamDyn's pitch actuator
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1136 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: e1a878a0d0eb769f1b2aa5454c22e846efa3ae19
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9350" uniqueCount="4733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9363" uniqueCount="4742">
   <si>
     <t>Category</t>
   </si>
@@ -14247,6 +14247,33 @@
   </si>
   <si>
     <t>(N-m/m)</t>
+  </si>
+  <si>
+    <t>Pitch Actuator</t>
+  </si>
+  <si>
+    <t>PAngInp</t>
+  </si>
+  <si>
+    <t>Pitch angle input</t>
+  </si>
+  <si>
+    <t>PAngAct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual pitch angle </t>
+  </si>
+  <si>
+    <t>PRatAct</t>
+  </si>
+  <si>
+    <t>PAccAct</t>
+  </si>
+  <si>
+    <t>Actual pitch rate</t>
+  </si>
+  <si>
+    <t>Actual pitch acceleration</t>
   </si>
 </sst>
 </file>
@@ -29323,10 +29350,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G354"/>
+  <dimension ref="A1:G359"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
+      <selection activeCell="E355" sqref="E355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34388,7 +34415,7 @@
         <v>4732</v>
       </c>
     </row>
-    <row r="353" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B353" t="s">
         <v>4729</v>
       </c>
@@ -34402,7 +34429,7 @@
         <v>4732</v>
       </c>
     </row>
-    <row r="354" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B354" t="s">
         <v>4730</v>
       </c>
@@ -34414,6 +34441,62 @@
       </c>
       <c r="F354" t="s">
         <v>4732</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A355" s="3" t="s">
+        <v>4733</v>
+      </c>
+      <c r="B355" s="3"/>
+      <c r="C355" s="6"/>
+      <c r="D355" s="6"/>
+      <c r="E355" s="6"/>
+      <c r="F355" s="3"/>
+      <c r="G355" s="3"/>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B356" s="4" t="s">
+        <v>4734</v>
+      </c>
+      <c r="D356" s="7" t="s">
+        <v>4735</v>
+      </c>
+      <c r="E356" s="7"/>
+      <c r="F356" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B357" t="s">
+        <v>4736</v>
+      </c>
+      <c r="D357" s="12" t="s">
+        <v>4737</v>
+      </c>
+      <c r="F357" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B358" t="s">
+        <v>4738</v>
+      </c>
+      <c r="D358" s="12" t="s">
+        <v>4740</v>
+      </c>
+      <c r="F358" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B359" t="s">
+        <v>4739</v>
+      </c>
+      <c r="D359" s="12" t="s">
+        <v>4741</v>
+      </c>
+      <c r="F359" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ updated version to 8.13.00 and added new TMD sources. + fixed issue in ReadFASTmesh.m where it didn't update the precision of the types I promoted to 8-byte realse in FAST 8.12. + updated conversion script to convert TMD input files
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1177 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: d0e79bcc5ac334ef2acba8cf2e77715ebe71a083
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/OutListParameters.xlsx
+++ b/modules-local/fast-library/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="420" windowWidth="11928" windowHeight="5304"/>
+    <workbookView xWindow="120" yWindow="420" windowWidth="11928" windowHeight="5304" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9360" uniqueCount="4739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9381" uniqueCount="4750">
   <si>
     <t>Category</t>
   </si>
@@ -14242,6 +14242,39 @@
   </si>
   <si>
     <t>Note that several outputs from FAST v7.2 are not yet implemented/available in FAST v8.12. See the worksheets labeled ("Removed")</t>
+  </si>
+  <si>
+    <t>Tower Tuned Mass Damper (TMD)</t>
+  </si>
+  <si>
+    <t>TTMD_XQ</t>
+  </si>
+  <si>
+    <t>TTMD_XQD</t>
+  </si>
+  <si>
+    <t>TTMD_YQ</t>
+  </si>
+  <si>
+    <t>TTMD_YQD</t>
+  </si>
+  <si>
+    <t>Tower X TMD position (displacement)</t>
+  </si>
+  <si>
+    <t>Tower X TMD velocity</t>
+  </si>
+  <si>
+    <t>Tower Y TMD position (displacement)</t>
+  </si>
+  <si>
+    <t>Tower Y TMD velocity</t>
+  </si>
+  <si>
+    <t>Relative to tower</t>
+  </si>
+  <si>
+    <t>.not. p%CompTTMD</t>
   </si>
 </sst>
 </file>
@@ -14691,7 +14724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -14734,7 +14767,7 @@
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="D9">
         <f>COUNTA(ServoDyn!B:B)-1</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
         <v>2066</v>
@@ -34461,10 +34494,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34705,7 +34738,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2078</v>
       </c>
@@ -34720,6 +34753,82 @@
       </c>
       <c r="G17" t="s">
         <v>2081</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>4739</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>4740</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4744</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2079</v>
+      </c>
+      <c r="F19" t="s">
+        <v>261</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>4741</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4745</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4748</v>
+      </c>
+      <c r="F20" t="s">
+        <v>491</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>4742</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4746</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2079</v>
+      </c>
+      <c r="F21" t="s">
+        <v>261</v>
+      </c>
+      <c r="G21" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>4743</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4747</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4748</v>
+      </c>
+      <c r="F22" t="s">
+        <v>491</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4749</v>
       </c>
     </row>
   </sheetData>
@@ -35038,7 +35147,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>352</v>
       </c>
@@ -35061,7 +35170,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>515</v>
       </c>
@@ -35069,7 +35178,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>242</v>
       </c>

</xml_diff>